<commit_message>
Updates to Pin Assignments
</commit_message>
<xml_diff>
--- a/tievox-hardware/Pin Assignments.xlsx
+++ b/tievox-hardware/Pin Assignments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="135">
   <si>
     <t>Pin</t>
   </si>
@@ -492,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -512,6 +512,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -796,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,9 +1120,8 @@
         <f>IF(ISERROR(VLOOKUP($A8,'GPIO Alts'!$A:$I,9,FALSE)),"",IF(VLOOKUP($A8,'GPIO Alts'!$A:$I,9,FALSE)=0, "", VLOOKUP($A8,'GPIO Alts'!$A:$I,9,FALSE)))</f>
         <v>ARM_TDI</v>
       </c>
-      <c r="I8" s="5" t="str">
-        <f>IF(ISERROR(VLOOKUP($A8,'GPIO Alts'!$A:$I,4,FALSE)),"",IF(VLOOKUP($A8,'GPIO Alts'!$A:$I,4,FALSE)=0, "", VLOOKUP($A8,'GPIO Alts'!$A:$I,4,FALSE)))</f>
-        <v>High</v>
+      <c r="I8" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>1</v>
@@ -2458,8 +2460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>